<commit_message>
Added documentation and addons
</commit_message>
<xml_diff>
--- a/Hardware/ESP32_Xmas_Star_Module/BOM_ESP32_Xmas_Star_Module.xlsx
+++ b/Hardware/ESP32_Xmas_Star_Module/BOM_ESP32_Xmas_Star_Module.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Library/CloudStorage/Dropbox/NADHack/Github-Repos/Xmas_Star2.0/Hardware/ESP32_Xmas_Star_Module/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81397EB1-4C18-6F43-817B-E8A19B9F43B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168447E0-0C18-0F48-9C54-223BA7BD89D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16860" xr2:uid="{10BD4B82-476F-8446-BE22-01B749018080}"/>
   </bookViews>
@@ -1100,7 +1100,7 @@
         <v>0.06</v>
       </c>
       <c r="J2">
-        <f>I2*B2</f>
+        <f t="shared" ref="J2:J8" si="0">I2*B2</f>
         <v>0.3</v>
       </c>
     </row>
@@ -1124,7 +1124,7 @@
         <v>0.03</v>
       </c>
       <c r="J3">
-        <f>I3*B3</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -1148,7 +1148,7 @@
         <v>1.57</v>
       </c>
       <c r="J4">
-        <f>I4*B4</f>
+        <f t="shared" si="0"/>
         <v>3.14</v>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
         <v>0.08</v>
       </c>
       <c r="J5">
-        <f>I5*B5</f>
+        <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
         <v>0.15</v>
       </c>
       <c r="J6">
-        <f>I6*B6</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="J7">
-        <f>I7*B7</f>
+        <f t="shared" si="0"/>
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -1244,7 +1244,7 @@
         <v>3.2</v>
       </c>
       <c r="J8">
-        <f>I8*B8</f>
+        <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
     </row>
@@ -1259,5 +1259,6 @@
     <hyperlink ref="F7" r:id="rId1" xr:uid="{198EB7A7-5FE5-8346-8C55-2562F084F718}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>